<commit_message>
add updates to a few comms/wimax related enforcements
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-05-23.xlsx
+++ b/EC/Train Runs and Enforcements 2016-05-23.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2059" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2062" uniqueCount="610">
   <si>
     <t>Train ID</t>
   </si>
@@ -1875,6 +1875,15 @@
   </si>
   <si>
     <t>Initialized, but never ran</t>
+  </si>
+  <si>
+    <t>http://stevetu21.github.io/eaglep3/load_kml.html?kml=http://rtdc.gmaps-snips.s3.amazonaws.com/1fbf74be-85f2-4e5d-ae4e-e56ecef6b6da.kml</t>
+  </si>
+  <si>
+    <t>http://stevetu21.github.io/eaglep3/load_kml.html?kml=http://rtdc.gmaps-snips.s3.amazonaws.com/ebe49858-27c6-44f3-b0fa-307a285f8863.kml</t>
+  </si>
+  <si>
+    <t>http://stevetu21.github.io/eaglep3/load_kml.html?kml=http://rtdc.gmaps-snips.s3.amazonaws.com/d7abf0c4-ee35-482c-ad86-a26a442f7c32.kml</t>
   </si>
 </sst>
 </file>
@@ -14697,7 +14706,7 @@
   <dimension ref="A1:R59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15522,7 +15531,7 @@
         <v>4008</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23">
         <v>42513.397546296299</v>
       </c>
@@ -15573,7 +15582,7 @@
         <v>4008</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23">
         <v>42513.398101851853</v>
       </c>
@@ -15624,7 +15633,7 @@
         <v>4008</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23">
         <v>42513.47079861111</v>
       </c>
@@ -15675,7 +15684,7 @@
         <v>4015</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <v>42513.546736111108</v>
       </c>
@@ -15726,7 +15735,7 @@
         <v>4008</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23">
         <v>42513.643923611111</v>
       </c>
@@ -15777,7 +15786,7 @@
         <v>4028</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23">
         <v>42514.052106481482</v>
       </c>
@@ -15828,7 +15837,7 @@
         <v>4007</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <v>42513.454942129632</v>
       </c>
@@ -15880,8 +15889,11 @@
         <f t="shared" si="0"/>
         <v>4027</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R23" s="83" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23">
         <v>42513.657141203701</v>
       </c>
@@ -15934,7 +15946,7 @@
         <v>4013</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <v>42513.769687499997</v>
       </c>
@@ -15987,7 +15999,7 @@
         <v>4014</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23">
         <v>42513.77138888889</v>
       </c>
@@ -16039,8 +16051,11 @@
         <f t="shared" si="0"/>
         <v>4020</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R26" s="83" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23">
         <v>42513.996296296296</v>
       </c>
@@ -16093,7 +16108,7 @@
         <v>4044</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23">
         <v>42513.661076388889</v>
       </c>
@@ -16145,8 +16160,11 @@
         <f t="shared" si="0"/>
         <v>4016</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R28" s="83" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
         <v>42513.269166666665</v>
       </c>
@@ -16197,7 +16215,7 @@
         <v>4028</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <v>42513.306307870371</v>
       </c>
@@ -16248,7 +16266,7 @@
         <v>4008</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23">
         <v>42513.320069444446</v>
       </c>
@@ -16299,7 +16317,7 @@
         <v>4041</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23">
         <v>42513.344849537039</v>
       </c>
@@ -17649,8 +17667,13 @@
       <formula>$M3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="R23" r:id="rId1"/>
+    <hyperlink ref="R28" r:id="rId2"/>
+    <hyperlink ref="R26" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>